<commit_message>
Translated from Danish to English
</commit_message>
<xml_diff>
--- a/Protocol_RX_To_TX.xlsx
+++ b/Protocol_RX_To_TX.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="16925"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="18201"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\57468\OneDrive_Personal\OneDrive\DYI Remote Control\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\57468\OneDrive_Personal\OneDrive\GitHub\DYI Remote Control\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -80,12 +80,6 @@
     <t>Byte 0</t>
   </si>
   <si>
-    <t>ID = Hvilken type pakke det er</t>
-  </si>
-  <si>
-    <t>Data 0-8 = Den data/talværdi der skal sendes</t>
-  </si>
-  <si>
     <t>Basic setup = 9 Bytes</t>
   </si>
   <si>
@@ -104,9 +98,6 @@
     <t>Ready?</t>
   </si>
   <si>
-    <t>Ready = spørg om modtageren er klar</t>
-  </si>
-  <si>
     <t>Braud rate</t>
   </si>
   <si>
@@ -137,15 +128,6 @@
     <t>00-03</t>
   </si>
   <si>
-    <t>Ved setup er 00 = don't care / bliv hvor du er</t>
-  </si>
-  <si>
-    <t>Div Protokol til RC RX til TX</t>
-  </si>
-  <si>
-    <t>Byte 1-4 = return hvor jeg er pt</t>
-  </si>
-  <si>
     <t>EF</t>
   </si>
   <si>
@@ -182,10 +164,28 @@
     <t>Vbatt</t>
   </si>
   <si>
-    <t>Vbatt = Analog værdig 00-FF eller 0-255</t>
-  </si>
-  <si>
     <t>s</t>
+  </si>
+  <si>
+    <t>ID = what packet type it is</t>
+  </si>
+  <si>
+    <t>Data 0-7 = the induvidual data that is being send</t>
+  </si>
+  <si>
+    <t>Vbatt = Analog value 00-FF(HEX) or 0-255(Binary)</t>
+  </si>
+  <si>
+    <t>At setup 00 = don't care / stay where you are</t>
+  </si>
+  <si>
+    <t>Ready = is the reciver ready / Booted?</t>
+  </si>
+  <si>
+    <t>Div Protocol for RC RX to TX</t>
+  </si>
+  <si>
+    <t>Byte 1-4 = return current setup</t>
   </si>
 </sst>
 </file>
@@ -485,11 +485,11 @@
     <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -851,7 +851,7 @@
   <dimension ref="B1:J69"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J11" sqref="J11"/>
+      <selection activeCell="O12" sqref="O12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -867,7 +867,7 @@
     <row r="1" spans="2:10" s="3" customFormat="1" x14ac:dyDescent="0.25"/>
     <row r="2" spans="2:10" s="2" customFormat="1" ht="27" thickBot="1" x14ac:dyDescent="0.45">
       <c r="B2" s="27" t="s">
-        <v>38</v>
+        <v>52</v>
       </c>
       <c r="C2" s="27"/>
       <c r="D2" s="27"/>
@@ -879,11 +879,11 @@
       <c r="J2" s="27"/>
     </row>
     <row r="4" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B4" s="24" t="s">
-        <v>20</v>
-      </c>
-      <c r="C4" s="24"/>
-      <c r="D4" s="24"/>
+      <c r="B4" s="25" t="s">
+        <v>18</v>
+      </c>
+      <c r="C4" s="25"/>
+      <c r="D4" s="25"/>
     </row>
     <row r="5" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="6" spans="2:10" x14ac:dyDescent="0.25">
@@ -957,7 +957,7 @@
     </row>
     <row r="9" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B9" s="29" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="C9" s="29"/>
       <c r="D9" s="29"/>
@@ -968,7 +968,7 @@
     </row>
     <row r="10" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B10" s="29" t="s">
-        <v>18</v>
+        <v>47</v>
       </c>
       <c r="C10" s="29"/>
       <c r="D10" s="29"/>
@@ -979,7 +979,7 @@
     </row>
     <row r="11" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B11" s="29" t="s">
-        <v>19</v>
+        <v>48</v>
       </c>
       <c r="C11" s="29"/>
       <c r="D11" s="29"/>
@@ -989,23 +989,23 @@
       <c r="H11" s="29"/>
     </row>
     <row r="12" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B12" s="25" t="s">
-        <v>24</v>
-      </c>
-      <c r="C12" s="25"/>
-      <c r="D12" s="25"/>
-      <c r="E12" s="25"/>
-      <c r="F12" s="25"/>
-      <c r="G12" s="25"/>
-      <c r="H12" s="25"/>
+      <c r="B12" s="29" t="s">
+        <v>22</v>
+      </c>
+      <c r="C12" s="29"/>
+      <c r="D12" s="29"/>
+      <c r="E12" s="29"/>
+      <c r="F12" s="29"/>
+      <c r="G12" s="29"/>
+      <c r="H12" s="29"/>
     </row>
     <row r="13" spans="2:10" s="1" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="15" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B15" s="24" t="s">
-        <v>43</v>
-      </c>
-      <c r="C15" s="24"/>
-      <c r="D15" s="24"/>
+      <c r="B15" s="25" t="s">
+        <v>37</v>
+      </c>
+      <c r="C15" s="25"/>
+      <c r="D15" s="25"/>
     </row>
     <row r="16" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="17" spans="2:10" x14ac:dyDescent="0.25">
@@ -1042,57 +1042,57 @@
         <v>8</v>
       </c>
       <c r="C18" s="13" t="s">
+        <v>24</v>
+      </c>
+      <c r="D18" s="13" t="s">
+        <v>25</v>
+      </c>
+      <c r="E18" s="13" t="s">
+        <v>26</v>
+      </c>
+      <c r="F18" s="13" t="s">
         <v>27</v>
       </c>
-      <c r="D18" s="13" t="s">
-        <v>28</v>
-      </c>
-      <c r="E18" s="13" t="s">
-        <v>29</v>
-      </c>
-      <c r="F18" s="13" t="s">
-        <v>30</v>
-      </c>
       <c r="G18" s="13" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="H18" s="13" t="s">
-        <v>51</v>
+        <v>45</v>
       </c>
       <c r="I18" s="13" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="J18" s="14" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
     </row>
     <row r="19" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B19" s="16" t="s">
-        <v>40</v>
+        <v>34</v>
       </c>
       <c r="C19" s="11" t="s">
+        <v>30</v>
+      </c>
+      <c r="D19" s="11" t="s">
+        <v>32</v>
+      </c>
+      <c r="E19" s="11" t="s">
+        <v>30</v>
+      </c>
+      <c r="F19" s="11" t="s">
         <v>33</v>
       </c>
-      <c r="D19" s="11" t="s">
-        <v>35</v>
-      </c>
-      <c r="E19" s="11" t="s">
-        <v>33</v>
-      </c>
-      <c r="F19" s="11" t="s">
-        <v>36</v>
-      </c>
       <c r="G19" s="11" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="H19" s="11" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="I19" s="11" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="J19" s="12" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
     </row>
     <row r="20" spans="2:10" x14ac:dyDescent="0.25">
@@ -1108,7 +1108,7 @@
     </row>
     <row r="21" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B21" s="26" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="C21" s="26"/>
       <c r="D21" s="26"/>
@@ -1121,7 +1121,7 @@
     </row>
     <row r="22" spans="2:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B22" s="26" t="s">
-        <v>37</v>
+        <v>50</v>
       </c>
       <c r="C22" s="26"/>
       <c r="D22" s="26"/>
@@ -1134,7 +1134,7 @@
     </row>
     <row r="23" spans="2:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B23" s="26" t="s">
-        <v>39</v>
+        <v>53</v>
       </c>
       <c r="C23" s="26"/>
       <c r="D23" s="26"/>
@@ -1169,7 +1169,7 @@
     </row>
     <row r="26" spans="2:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B26" s="30" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="C26" s="30"/>
       <c r="D26" s="20"/>
@@ -1225,57 +1225,57 @@
         <v>8</v>
       </c>
       <c r="C29" s="13" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="D29" s="13" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="E29" s="13" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="F29" s="13" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="G29" s="13" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="H29" s="13" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="I29" s="13" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="J29" s="14" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
     </row>
     <row r="30" spans="2:10" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B30" s="16" t="s">
-        <v>41</v>
+        <v>35</v>
       </c>
       <c r="C30" s="11" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="D30" s="11" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="E30" s="11" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="F30" s="11" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="G30" s="11" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="H30" s="11" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="I30" s="11" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="J30" s="12" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
     </row>
     <row r="31" spans="2:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -1291,7 +1291,7 @@
     </row>
     <row r="32" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B32" s="28" t="s">
-        <v>26</v>
+        <v>51</v>
       </c>
       <c r="C32" s="28"/>
       <c r="D32" s="28"/>
@@ -1302,12 +1302,12 @@
     </row>
     <row r="33" spans="2:10" s="1" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="35" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B35" s="24" t="s">
-        <v>44</v>
-      </c>
-      <c r="C35" s="24"/>
+      <c r="B35" s="25" t="s">
+        <v>38</v>
+      </c>
+      <c r="C35" s="25"/>
       <c r="J35" t="s">
-        <v>53</v>
+        <v>46</v>
       </c>
     </row>
     <row r="36" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
@@ -1345,74 +1345,74 @@
         <v>8</v>
       </c>
       <c r="C38" s="13" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="D38" s="13" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="E38" s="13" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="F38" s="13" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="G38" s="13" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="H38" s="13" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="I38" s="13" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="J38" s="14" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
     </row>
     <row r="39" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B39" s="16" t="s">
-        <v>42</v>
+        <v>36</v>
       </c>
       <c r="C39" s="11" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="D39" s="11" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="E39" s="11" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="F39" s="11" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="G39" s="11" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="H39" s="11" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="I39" s="11" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="J39" s="12" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
     </row>
     <row r="41" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B41" s="25"/>
-      <c r="C41" s="25"/>
-      <c r="D41" s="25"/>
-      <c r="E41" s="25"/>
-      <c r="F41" s="25"/>
-      <c r="G41" s="25"/>
-      <c r="H41" s="25"/>
+      <c r="B41" s="24"/>
+      <c r="C41" s="24"/>
+      <c r="D41" s="24"/>
+      <c r="E41" s="24"/>
+      <c r="F41" s="24"/>
+      <c r="G41" s="24"/>
+      <c r="H41" s="24"/>
     </row>
     <row r="42" spans="2:10" s="1" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="44" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B44" s="24" t="s">
-        <v>45</v>
-      </c>
-      <c r="C44" s="24"/>
+      <c r="B44" s="25" t="s">
+        <v>39</v>
+      </c>
+      <c r="C44" s="25"/>
     </row>
     <row r="45" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="46" spans="2:10" x14ac:dyDescent="0.25">
@@ -1449,74 +1449,74 @@
         <v>8</v>
       </c>
       <c r="C47" s="13" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="D47" s="13" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="E47" s="13" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="F47" s="13" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="G47" s="13" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="H47" s="13" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="I47" s="13" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="J47" s="14" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
     </row>
     <row r="48" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B48" s="16" t="s">
-        <v>48</v>
+        <v>42</v>
       </c>
       <c r="C48" s="11" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="D48" s="11" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="E48" s="11" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="F48" s="11" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="G48" s="11" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="H48" s="11" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="I48" s="11" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="J48" s="12" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
     </row>
     <row r="50" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B50" s="25"/>
-      <c r="C50" s="25"/>
-      <c r="D50" s="25"/>
-      <c r="E50" s="25"/>
-      <c r="F50" s="25"/>
-      <c r="G50" s="25"/>
-      <c r="H50" s="25"/>
+      <c r="B50" s="24"/>
+      <c r="C50" s="24"/>
+      <c r="D50" s="24"/>
+      <c r="E50" s="24"/>
+      <c r="F50" s="24"/>
+      <c r="G50" s="24"/>
+      <c r="H50" s="24"/>
     </row>
     <row r="51" spans="2:10" s="1" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="53" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B53" s="24" t="s">
-        <v>46</v>
-      </c>
-      <c r="C53" s="24"/>
+      <c r="B53" s="25" t="s">
+        <v>40</v>
+      </c>
+      <c r="C53" s="25"/>
     </row>
     <row r="54" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="55" spans="2:10" x14ac:dyDescent="0.25">
@@ -1553,74 +1553,74 @@
         <v>8</v>
       </c>
       <c r="C56" s="13" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="D56" s="13" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="E56" s="13" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="F56" s="13" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="G56" s="13" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="H56" s="13" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="I56" s="13" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="J56" s="14" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
     </row>
     <row r="57" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B57" s="16" t="s">
-        <v>49</v>
+        <v>43</v>
       </c>
       <c r="C57" s="11" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="D57" s="11" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="E57" s="11" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="F57" s="11" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="G57" s="11" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="H57" s="11" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="I57" s="11" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="J57" s="12" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
     </row>
     <row r="59" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B59" s="25"/>
-      <c r="C59" s="25"/>
-      <c r="D59" s="25"/>
-      <c r="E59" s="25"/>
-      <c r="F59" s="25"/>
-      <c r="G59" s="25"/>
-      <c r="H59" s="25"/>
+      <c r="B59" s="24"/>
+      <c r="C59" s="24"/>
+      <c r="D59" s="24"/>
+      <c r="E59" s="24"/>
+      <c r="F59" s="24"/>
+      <c r="G59" s="24"/>
+      <c r="H59" s="24"/>
     </row>
     <row r="60" spans="2:10" s="1" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="62" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B62" s="24" t="s">
-        <v>47</v>
-      </c>
-      <c r="C62" s="24"/>
+      <c r="B62" s="25" t="s">
+        <v>41</v>
+      </c>
+      <c r="C62" s="25"/>
     </row>
     <row r="63" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="64" spans="2:10" x14ac:dyDescent="0.25">
@@ -1657,71 +1657,73 @@
         <v>8</v>
       </c>
       <c r="C65" s="13" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="D65" s="13" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="E65" s="13" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="F65" s="13" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="G65" s="13" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="H65" s="13" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="I65" s="13" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="J65" s="14" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
     </row>
     <row r="66" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B66" s="16" t="s">
-        <v>50</v>
+        <v>44</v>
       </c>
       <c r="C66" s="11" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="D66" s="11" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="E66" s="11" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="F66" s="11" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="G66" s="11" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="H66" s="11" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="I66" s="11" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="J66" s="12" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
     </row>
     <row r="68" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B68" s="25"/>
-      <c r="C68" s="25"/>
-      <c r="D68" s="25"/>
-      <c r="E68" s="25"/>
-      <c r="F68" s="25"/>
-      <c r="G68" s="25"/>
-      <c r="H68" s="25"/>
+      <c r="B68" s="24"/>
+      <c r="C68" s="24"/>
+      <c r="D68" s="24"/>
+      <c r="E68" s="24"/>
+      <c r="F68" s="24"/>
+      <c r="G68" s="24"/>
+      <c r="H68" s="24"/>
     </row>
     <row r="69" spans="2:10" s="1" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
   </sheetData>
   <mergeCells count="20">
+    <mergeCell ref="B21:H21"/>
+    <mergeCell ref="B53:C53"/>
     <mergeCell ref="B2:J2"/>
     <mergeCell ref="B4:D4"/>
     <mergeCell ref="B12:H12"/>
@@ -1733,15 +1735,13 @@
     <mergeCell ref="B26:C26"/>
     <mergeCell ref="B22:H22"/>
     <mergeCell ref="B15:D15"/>
-    <mergeCell ref="B41:H41"/>
-    <mergeCell ref="B44:C44"/>
-    <mergeCell ref="B50:H50"/>
-    <mergeCell ref="B21:H21"/>
-    <mergeCell ref="B53:C53"/>
     <mergeCell ref="B59:H59"/>
     <mergeCell ref="B62:C62"/>
     <mergeCell ref="B68:H68"/>
     <mergeCell ref="B35:C35"/>
+    <mergeCell ref="B41:H41"/>
+    <mergeCell ref="B44:C44"/>
+    <mergeCell ref="B50:H50"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
More Protocol with working packet type detection
</commit_message>
<xml_diff>
--- a/Protocol_RX_To_TX.xlsx
+++ b/Protocol_RX_To_TX.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="197" uniqueCount="54">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="196" uniqueCount="53">
   <si>
     <t>Byte 1</t>
   </si>
@@ -128,9 +128,6 @@
     <t>00-03</t>
   </si>
   <si>
-    <t>EF</t>
-  </si>
-  <si>
     <t>EE</t>
   </si>
   <si>
@@ -164,9 +161,6 @@
     <t>Vbatt</t>
   </si>
   <si>
-    <t>s</t>
-  </si>
-  <si>
     <t>ID = what packet type it is</t>
   </si>
   <si>
@@ -186,6 +180,9 @@
   </si>
   <si>
     <t>Byte 1-4 = return current setup</t>
+  </si>
+  <si>
+    <t>E9</t>
   </si>
 </sst>
 </file>
@@ -497,10 +494,10 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -850,8 +847,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:J69"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="O12" sqref="O12"/>
+    <sheetView tabSelected="1" topLeftCell="A44" workbookViewId="0">
+      <selection activeCell="B66" sqref="B66"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -867,7 +864,7 @@
     <row r="1" spans="2:10" s="3" customFormat="1" x14ac:dyDescent="0.25"/>
     <row r="2" spans="2:10" s="2" customFormat="1" ht="27" thickBot="1" x14ac:dyDescent="0.45">
       <c r="B2" s="27" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="C2" s="27"/>
       <c r="D2" s="27"/>
@@ -956,53 +953,53 @@
       <c r="J8" s="4"/>
     </row>
     <row r="9" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B9" s="29" t="s">
+      <c r="B9" s="28" t="s">
         <v>20</v>
       </c>
-      <c r="C9" s="29"/>
-      <c r="D9" s="29"/>
-      <c r="E9" s="29"/>
-      <c r="F9" s="29"/>
-      <c r="G9" s="29"/>
-      <c r="H9" s="29"/>
+      <c r="C9" s="28"/>
+      <c r="D9" s="28"/>
+      <c r="E9" s="28"/>
+      <c r="F9" s="28"/>
+      <c r="G9" s="28"/>
+      <c r="H9" s="28"/>
     </row>
     <row r="10" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B10" s="29" t="s">
-        <v>47</v>
-      </c>
-      <c r="C10" s="29"/>
-      <c r="D10" s="29"/>
-      <c r="E10" s="29"/>
-      <c r="F10" s="29"/>
-      <c r="G10" s="29"/>
-      <c r="H10" s="29"/>
+      <c r="B10" s="28" t="s">
+        <v>45</v>
+      </c>
+      <c r="C10" s="28"/>
+      <c r="D10" s="28"/>
+      <c r="E10" s="28"/>
+      <c r="F10" s="28"/>
+      <c r="G10" s="28"/>
+      <c r="H10" s="28"/>
     </row>
     <row r="11" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B11" s="29" t="s">
-        <v>48</v>
-      </c>
-      <c r="C11" s="29"/>
-      <c r="D11" s="29"/>
-      <c r="E11" s="29"/>
-      <c r="F11" s="29"/>
-      <c r="G11" s="29"/>
-      <c r="H11" s="29"/>
+      <c r="B11" s="28" t="s">
+        <v>46</v>
+      </c>
+      <c r="C11" s="28"/>
+      <c r="D11" s="28"/>
+      <c r="E11" s="28"/>
+      <c r="F11" s="28"/>
+      <c r="G11" s="28"/>
+      <c r="H11" s="28"/>
     </row>
     <row r="12" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B12" s="29" t="s">
+      <c r="B12" s="28" t="s">
         <v>22</v>
       </c>
-      <c r="C12" s="29"/>
-      <c r="D12" s="29"/>
-      <c r="E12" s="29"/>
-      <c r="F12" s="29"/>
-      <c r="G12" s="29"/>
-      <c r="H12" s="29"/>
+      <c r="C12" s="28"/>
+      <c r="D12" s="28"/>
+      <c r="E12" s="28"/>
+      <c r="F12" s="28"/>
+      <c r="G12" s="28"/>
+      <c r="H12" s="28"/>
     </row>
     <row r="13" spans="2:10" s="1" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="15" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B15" s="25" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C15" s="25"/>
       <c r="D15" s="25"/>
@@ -1057,7 +1054,7 @@
         <v>31</v>
       </c>
       <c r="H18" s="13" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="I18" s="13" t="s">
         <v>21</v>
@@ -1108,7 +1105,7 @@
     </row>
     <row r="21" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B21" s="26" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="C21" s="26"/>
       <c r="D21" s="26"/>
@@ -1121,7 +1118,7 @@
     </row>
     <row r="22" spans="2:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B22" s="26" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="C22" s="26"/>
       <c r="D22" s="26"/>
@@ -1134,7 +1131,7 @@
     </row>
     <row r="23" spans="2:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B23" s="26" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="C23" s="26"/>
       <c r="D23" s="26"/>
@@ -1290,25 +1287,22 @@
       <c r="J31" s="19"/>
     </row>
     <row r="32" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B32" s="28" t="s">
-        <v>51</v>
-      </c>
-      <c r="C32" s="28"/>
-      <c r="D32" s="28"/>
-      <c r="E32" s="28"/>
-      <c r="F32" s="28"/>
-      <c r="G32" s="28"/>
-      <c r="H32" s="28"/>
+      <c r="B32" s="29" t="s">
+        <v>49</v>
+      </c>
+      <c r="C32" s="29"/>
+      <c r="D32" s="29"/>
+      <c r="E32" s="29"/>
+      <c r="F32" s="29"/>
+      <c r="G32" s="29"/>
+      <c r="H32" s="29"/>
     </row>
     <row r="33" spans="2:10" s="1" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="35" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B35" s="25" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C35" s="25"/>
-      <c r="J35" t="s">
-        <v>46</v>
-      </c>
     </row>
     <row r="36" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="37" spans="2:10" x14ac:dyDescent="0.25">
@@ -1371,7 +1365,7 @@
     </row>
     <row r="39" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B39" s="16" t="s">
-        <v>36</v>
+        <v>41</v>
       </c>
       <c r="C39" s="11" t="s">
         <v>19</v>
@@ -1410,7 +1404,7 @@
     <row r="42" spans="2:10" s="1" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="44" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B44" s="25" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C44" s="25"/>
     </row>
@@ -1514,7 +1508,7 @@
     <row r="51" spans="2:10" s="1" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="53" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B53" s="25" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C53" s="25"/>
     </row>
@@ -1618,7 +1612,7 @@
     <row r="60" spans="2:10" s="1" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="62" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B62" s="25" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C62" s="25"/>
     </row>
@@ -1683,7 +1677,7 @@
     </row>
     <row r="66" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B66" s="16" t="s">
-        <v>44</v>
+        <v>52</v>
       </c>
       <c r="C66" s="11" t="s">
         <v>19</v>

</xml_diff>